<commit_message>
fix bug 12 desember
</commit_message>
<xml_diff>
--- a/uploads/template_users.xlsx
+++ b/uploads/template_users.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>First Name</t>
   </si>
@@ -44,22 +44,25 @@
     <t>Category</t>
   </si>
   <si>
-    <t>guru1</t>
-  </si>
-  <si>
-    <t>guru1@tes.com</t>
-  </si>
-  <si>
-    <t>guru2</t>
-  </si>
-  <si>
-    <t>guru3</t>
-  </si>
-  <si>
-    <t>guru2@tes.com</t>
-  </si>
-  <si>
-    <t>guru3@tes.com</t>
+    <t>guru</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>mtk</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>gurubin@tes.com</t>
+  </si>
+  <si>
+    <t>gurumtk@tes.com</t>
+  </si>
+  <si>
+    <t>gurubig@tes.com</t>
   </si>
   <si>
     <t>siswa1</t>
@@ -87,39 +90,6 @@
   </si>
   <si>
     <t>siswa9</t>
-  </si>
-  <si>
-    <t>siswa10</t>
-  </si>
-  <si>
-    <t>siswa11</t>
-  </si>
-  <si>
-    <t>siswa12</t>
-  </si>
-  <si>
-    <t>siswa13</t>
-  </si>
-  <si>
-    <t>siswa14</t>
-  </si>
-  <si>
-    <t>siswa15</t>
-  </si>
-  <si>
-    <t>siswa16</t>
-  </si>
-  <si>
-    <t>siswa17</t>
-  </si>
-  <si>
-    <t>siswa18</t>
-  </si>
-  <si>
-    <t>siswa19</t>
-  </si>
-  <si>
-    <t>siswa20</t>
   </si>
 </sst>
 </file>
@@ -448,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F6" sqref="F6:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,8 +453,11 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>12345678</v>
@@ -495,10 +468,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>12345678</v>
@@ -509,10 +485,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>12345678</v>
@@ -523,7 +502,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
       </c>
       <c r="C5" t="str">
         <f>A5&amp;"@tes.com"</f>
@@ -538,10 +520,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:C24" si="0">A6&amp;"@tes.com"</f>
+        <f t="shared" ref="C6:C13" si="0">A6&amp;"@tes.com"</f>
         <v>siswa2@tes.com</v>
       </c>
       <c r="D6">
@@ -553,7 +538,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -568,7 +556,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -583,7 +574,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -598,7 +592,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -613,7 +610,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -628,7 +628,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -643,7 +646,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -653,171 +659,6 @@
         <v>12345678</v>
       </c>
       <c r="F13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa10@tes.com</v>
-      </c>
-      <c r="D14">
-        <v>12345678</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa11@tes.com</v>
-      </c>
-      <c r="D15">
-        <v>12345678</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa12@tes.com</v>
-      </c>
-      <c r="D16">
-        <v>12345678</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa13@tes.com</v>
-      </c>
-      <c r="D17">
-        <v>12345678</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa14@tes.com</v>
-      </c>
-      <c r="D18">
-        <v>12345678</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa15@tes.com</v>
-      </c>
-      <c r="D19">
-        <v>12345678</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa16@tes.com</v>
-      </c>
-      <c r="D20">
-        <v>12345678</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa17@tes.com</v>
-      </c>
-      <c r="D21">
-        <v>12345678</v>
-      </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa18@tes.com</v>
-      </c>
-      <c r="D22">
-        <v>12345678</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa19@tes.com</v>
-      </c>
-      <c r="D23">
-        <v>12345678</v>
-      </c>
-      <c r="F23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>siswa20@tes.com</v>
-      </c>
-      <c r="D24">
-        <v>12345678</v>
-      </c>
-      <c r="F24">
         <v>3</v>
       </c>
     </row>
@@ -833,6 +674,5 @@
     <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>